<commit_message>
MODIFIED: ExcelUtil class readData method
</commit_message>
<xml_diff>
--- a/build/resources/test/UdemyApplicationData.xlsx
+++ b/build/resources/test/UdemyApplicationData.xlsx
@@ -25,9 +25,6 @@
     <t>dineshkumar.icon@gmail.com</t>
   </si>
   <si>
-    <t>Dinnu@247</t>
-  </si>
-  <si>
     <t>dineshkumar.icon.dk@gmail.com</t>
   </si>
   <si>
@@ -35,6 +32,9 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>din1256jlgr</t>
   </si>
 </sst>
 </file>
@@ -366,7 +366,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -377,10 +377,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -388,15 +388,15 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -404,15 +404,15 @@
         <v>0</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -420,15 +420,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -436,15 +436,15 @@
         <v>0</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -452,15 +452,15 @@
         <v>0</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -468,15 +468,15 @@
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -497,29 +497,19 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="B2" r:id="rId2" display="Dinnu@247"/>
     <hyperlink ref="A3" r:id="rId3"/>
-    <hyperlink ref="B3" r:id="rId4"/>
-    <hyperlink ref="A4" r:id="rId5"/>
-    <hyperlink ref="B4" r:id="rId6"/>
-    <hyperlink ref="A5" r:id="rId7"/>
-    <hyperlink ref="B5" r:id="rId8"/>
-    <hyperlink ref="A6" r:id="rId9"/>
-    <hyperlink ref="B6" r:id="rId10"/>
-    <hyperlink ref="A7" r:id="rId11"/>
-    <hyperlink ref="B7" r:id="rId12"/>
-    <hyperlink ref="A8" r:id="rId13"/>
-    <hyperlink ref="B8" r:id="rId14"/>
-    <hyperlink ref="A9" r:id="rId15"/>
-    <hyperlink ref="B9" r:id="rId16"/>
-    <hyperlink ref="A10" r:id="rId17"/>
-    <hyperlink ref="A12" r:id="rId18"/>
-    <hyperlink ref="B10" r:id="rId19"/>
-    <hyperlink ref="B12" r:id="rId20"/>
-    <hyperlink ref="A11" r:id="rId21"/>
-    <hyperlink ref="A13" r:id="rId22"/>
-    <hyperlink ref="B11" r:id="rId23"/>
-    <hyperlink ref="B13" r:id="rId24"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A5" r:id="rId5"/>
+    <hyperlink ref="A6" r:id="rId6"/>
+    <hyperlink ref="A7" r:id="rId7"/>
+    <hyperlink ref="A8" r:id="rId8"/>
+    <hyperlink ref="A9" r:id="rId9"/>
+    <hyperlink ref="A10" r:id="rId10"/>
+    <hyperlink ref="A12" r:id="rId11"/>
+    <hyperlink ref="A11" r:id="rId12"/>
+    <hyperlink ref="A13" r:id="rId13"/>
+    <hyperlink ref="B3:B13" r:id="rId14" display="Dinnu@247"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>